<commit_message>
test: correct the excel file to import test
</commit_message>
<xml_diff>
--- a/tests/Stubs/products-import-file.xlsx
+++ b/tests/Stubs/products-import-file.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t xml:space="preserve">EAN</t>
   </si>
@@ -34,7 +34,7 @@
     <t xml:space="preserve">DESCRIPCION</t>
   </si>
   <si>
-    <t xml:space="preserve">ID_CATEGORIA</t>
+    <t xml:space="preserve">CATEGORIA</t>
   </si>
   <si>
     <t xml:space="preserve">PRECIO</t>
@@ -53,6 +53,12 @@
   </si>
   <si>
     <t xml:space="preserve">A fake description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Categoria test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11/01/2020</t>
   </si>
 </sst>
 </file>
@@ -64,7 +70,7 @@
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="166" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -85,6 +91,12 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="0"/>
     </font>
   </fonts>
@@ -143,7 +155,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -167,7 +179,7 @@
   <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -216,8 +228,8 @@
       <c r="D2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="0" t="n">
-        <v>1</v>
+      <c r="E2" s="0" t="s">
+        <v>11</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>999999</v>
@@ -225,8 +237,8 @@
       <c r="G2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="H2" s="3" t="n">
-        <v>44146</v>
+      <c r="H2" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>